<commit_message>
almost done replacement by panautogui is remaining
</commit_message>
<xml_diff>
--- a/output_results.xlsx
+++ b/output_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,7 +514,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0TlRjNE5EaG1OaTFpTkRRNExUUXlPREV0T0RGaE5TMWxNamt3TXpNeFpUa3laR0lRQVE9PRAIGiQwQzY5MDE0QS00MzJDLTRBMkUtQjM2QS00RTUxRjEwMjNCRDU</t>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrWm1RMFlUZ3hOaTFtWlRNMkxUUXdORGN0T0dGbU9TMHpZelpoTkRKaVl6Y3labVVRQVE9PRAIGiRENUU4OUJFQi04NzhFLTQ3N0ItODlGMC0wMkQ2RjkxMjdGREI</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0TlRjNE5EaG1OaTFpTkRRNExUUXlPREV0T0RGaE5TMWxNamt3TXpNeFpUa3laR0lRQVE9PRAIGiQwQzY5MDE0QS00MzJDLTRBMkUtQjM2QS00RTUxRjEwMjNCRDU</t>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrWm1RMFlUZ3hOaTFtWlRNMkxUUXdORGN0T0dGbU9TMHpZelpoTkRKaVl6Y3labVVRQVE9PRAIGiRENUU4OUJFQi04NzhFLTQ3N0ItODlGMC0wMkQ2RjkxMjdGREI</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0TlRjNE5EaG1OaTFpTkRRNExUUXlPREV0T0RGaE5TMWxNamt3TXpNeFpUa3laR0lRQVE9PRAIGiQwQzY5MDE0QS00MzJDLTRBMkUtQjM2QS00RTUxRjEwMjNCRDU</t>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrWm1RMFlUZ3hOaTFtWlRNMkxUUXdORGN0T0dGbU9TMHpZelpoTkRKaVl6Y3labVVRQVE9PRAIGiRENUU4OUJFQi04NzhFLTQ3N0ItODlGMC0wMkQ2RjkxMjdGREI</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -544,10 +544,126 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0TlRjNE5EaG1OaTFpTkRRNExUUXlPREV0T0RGaE5TMWxNamt3TXpNeFpUa3laR0lRQVE9PRAIGiQwQzY5MDE0QS00MzJDLTRBMkUtQjM2QS00RTUxRjEwMjNCRDU</t>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrWm1RMFlUZ3hOaTFtWlRNMkxUUXdORGN0T0dGbU9TMHpZelpoTkRKaVl6Y3labVVRQVE9PRAIGiRENUU4OUJFQi04NzhFLTQ3N0ItODlGMC0wMkQ2RjkxMjdGREI</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Free: Debian, CentOS, CoreOS, Ubuntu or BY</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>general purpose</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTXpkbVpUazROaTFpTldOa0xUUXhZek10T0dJd09TMWtNVGxoTVdVMFlqRTBPV1VRQVE9PRAIGiQ2RkNCRThFRi03OUI4LTRFOUYtODcxRS1EODg3NjhEMTc3QkU</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTXpkbVpUazROaTFpTldOa0xUUXhZek10T0dJd09TMWtNVGxoTVdVMFlqRTBPV1VRQVE9PRAIGiQ2RkNCRThFRi03OUI4LTRFOUYtODcxRS1EODg3NjhEMTc3QkU</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTXpkbVpUazROaTFpTldOa0xUUXhZek10T0dJd09TMWtNVGxoTVdVMFlqRTBPV1VRQVE9PRAIGiQ2RkNCRThFRi03OUI4LTRFOUYtODcxRS1EODg3NjhEMTc3QkU</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTXpkbVpUazROaTFpTldOa0xUUXhZek10T0dJd09TMWtNVGxoTVdVMFlqRTBPV1VRQVE9PRAIGiQ2RkNCRThFRi03OUI4LTRFOUYtODcxRS1EODg3NjhEMTc3QkU</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Free: Debian, CentOS, CoreOS, Ubuntu or BY</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>general purpose</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3WXpCbE9EZGlNUzB4WTJFeUxUUTROVEl0WW1VMk9DMWtZVE16TWpReE9HVTVZalFRQVE9PRAIGiRFMUY2OTVEQy03NjExLTQ3MzktOTBFNC0zMzVDQjIyMzk3NTc</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3WXpCbE9EZGlNUzB4WTJFeUxUUTROVEl0WW1VMk9DMWtZVE16TWpReE9HVTVZalFRQVE9PRAIGiRFMUY2OTVEQy03NjExLTQ3MzktOTBFNC0zMzVDQjIyMzk3NTc</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3WXpCbE9EZGlNUzB4WTJFeUxUUTROVEl0WW1VMk9DMWtZVE16TWpReE9HVTVZalFRQVE9PRAIGiRFMUY2OTVEQy03NjExLTQ3MzktOTBFNC0zMzVDQjIyMzk3NTc</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3WXpCbE9EZGlNUzB4WTJFeUxUUTROVEl0WW1VMk9DMWtZVE16TWpReE9HVTVZalFRQVE9PRAIGiRFMUY2OTVEQy03NjExLTQ3MzktOTBFNC0zMzVDQjIyMzk3NTc</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>$8.54</t>
         </is>

</xml_diff>